<commit_message>
Adding initial OMP script, cleaned up notebook, and updated results.
</commit_message>
<xml_diff>
--- a/TP_Results.xlsx
+++ b/TP_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Development/CSC746/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1201429-13C0-7749-83E3-9E5638524A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727B8B1F-B3B2-2D4F-865B-134F06CDDCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9940" yWindow="1920" windowWidth="27960" windowHeight="20940" xr2:uid="{65D3B227-0E49-8B43-81E6-D1DC9C42394E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>MacBookPro</t>
   </si>
@@ -72,7 +72,39 @@
     <t>10/10 9:00AM</t>
   </si>
   <si>
-    <t>10/10 9:10AM</t>
+    <t>RandomizedSearchCV</t>
+  </si>
+  <si>
+    <t>n_iter</t>
+  </si>
+  <si>
+    <t>cv_folds</t>
+  </si>
+  <si>
+    <t>elapsed_time</t>
+  </si>
+  <si>
+    <t>{'n_estimators': 600,
+ 'min_samples_split': 2,
+ 'min_samples_leaf': 2,
+ 'max_features': 'auto',
+ 'max_depth': 60,
+ 'bootstrap': False}</t>
+  </si>
+  <si>
+    <t>best_params</t>
+  </si>
+  <si>
+    <t>min_samples_split</t>
+  </si>
+  <si>
+    <t>min_samples_leaf</t>
+  </si>
+  <si>
+    <t>max_depth</t>
+  </si>
+  <si>
+    <t>10/10 2:15PM</t>
   </si>
 </sst>
 </file>
@@ -110,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,6 +161,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,12 +180,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DF7997-F2CF-2F45-80A2-37163737BEBC}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" style="1" customWidth="1"/>
@@ -479,10 +522,11 @@
     <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="36.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,13 +540,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
@@ -519,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100</v>
       </c>
@@ -539,24 +589,72 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>100</v>
+        <v>600</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G5" s="1">
-        <v>303.01866000000001</v>
+        <v>199.09338</v>
       </c>
       <c r="H5" s="1">
-        <v>0.97106999999999999</v>
+        <v>0.97228999999999999</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2287.3885500000001</v>
+      </c>
+      <c r="I12" s="5">
+        <v>44479.583333333336</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>